<commit_message>
edited processing and reprocessing function
</commit_message>
<xml_diff>
--- a/DNA_v2/DNA_assay/DNA74/abs_reading.xlsx
+++ b/DNA_v2/DNA_assay/DNA74/abs_reading.xlsx
@@ -1,13 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView xWindow="204" yWindow="588" windowWidth="22716" windowHeight="8676" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="General" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Plate1" sheetId="2" r:id="rId5"/>
+    <sheet name="General" sheetId="1" r:id="rId1"/>
+    <sheet name="Plate1" sheetId="2" r:id="rId2"/>
+    <sheet name="Plate2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="EAra6BXNCRU5BtyTJMG9qP6vp4prKWdFTarUagMNFGE="/>
@@ -17,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="106">
   <si>
     <t>User</t>
   </si>
@@ -340,22 +344,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arimo"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arimo"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arimo"/>
     </font>
@@ -365,46 +369,47 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -594,23 +599,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B991"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="27.71"/>
+    <col min="1" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.0" customHeight="1">
+    <row r="1" spans="1:2" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.0" customHeight="1">
+    <row r="2" spans="1:2" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -626,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="15.0" customHeight="1">
+    <row r="3" spans="1:2" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -634,7 +639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="15.0" customHeight="1">
+    <row r="4" spans="1:2" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -642,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="15.0" customHeight="1">
+    <row r="5" spans="1:2" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -650,7 +655,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="15.0" customHeight="1">
+    <row r="6" spans="1:2" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -658,7 +663,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="15.0" customHeight="1">
+    <row r="7" spans="1:2" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -666,7 +671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" ht="15.0" customHeight="1">
+    <row r="8" spans="1:2" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -674,7 +679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="15.0" customHeight="1">
+    <row r="9" spans="1:2" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -682,13 +687,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="12.75" customHeight="1"/>
-    <row r="11" ht="15.0" customHeight="1">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="11" spans="1:2" ht="15" customHeight="1">
+      <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" ht="15.0" customHeight="1">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -696,13 +702,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" ht="12.75" customHeight="1"/>
-    <row r="14" ht="15.0" customHeight="1">
-      <c r="A14" s="1" t="s">
+    <row r="13" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="14" spans="1:2" ht="15" customHeight="1">
+      <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" ht="15.0" customHeight="1">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -710,7 +717,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" ht="15.0" customHeight="1">
+    <row r="16" spans="1:2" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
@@ -718,7 +725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" ht="15.0" customHeight="1">
+    <row r="17" spans="1:2" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -726,7 +733,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" ht="15.0" customHeight="1">
+    <row r="18" spans="1:2" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -734,7 +741,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" ht="15.0" customHeight="1">
+    <row r="19" spans="1:2" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -742,7 +749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" ht="15.0" customHeight="1">
+    <row r="20" spans="1:2" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -750,7 +757,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" ht="15.0" customHeight="1">
+    <row r="21" spans="1:2" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -758,7 +765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" ht="15.0" customHeight="1">
+    <row r="22" spans="1:2" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
@@ -766,7 +773,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" ht="15.0" customHeight="1">
+    <row r="23" spans="1:2" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>37</v>
       </c>
@@ -774,7 +781,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" ht="15.0" customHeight="1">
+    <row r="24" spans="1:2" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -782,7 +789,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" ht="15.0" customHeight="1">
+    <row r="25" spans="1:2" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -790,13 +797,14 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" ht="12.75" customHeight="1"/>
-    <row r="27" ht="15.0" customHeight="1">
-      <c r="A27" s="1" t="s">
+    <row r="26" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="27" spans="1:2" ht="15" customHeight="1">
+      <c r="A27" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" ht="15.0" customHeight="1">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -804,7 +812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" ht="15.0" customHeight="1">
+    <row r="29" spans="1:2" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
@@ -812,13 +820,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" ht="12.75" customHeight="1"/>
-    <row r="31" ht="15.0" customHeight="1">
-      <c r="A31" s="1" t="s">
+    <row r="30" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="31" spans="1:2" ht="15" customHeight="1">
+      <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" ht="15.0" customHeight="1">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:2" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -826,7 +835,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" ht="15.0" customHeight="1">
+    <row r="33" spans="1:2" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
@@ -834,13 +843,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" ht="12.75" customHeight="1"/>
-    <row r="35" ht="15.0" customHeight="1">
-      <c r="A35" s="1" t="s">
+    <row r="34" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="35" spans="1:2" ht="15" customHeight="1">
+      <c r="A35" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" ht="15.0" customHeight="1">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="1:2" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>44</v>
       </c>
@@ -848,7 +858,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" ht="15.0" customHeight="1">
+    <row r="37" spans="1:2" ht="15" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
@@ -856,13 +866,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" ht="12.75" customHeight="1"/>
-    <row r="39" ht="15.0" customHeight="1">
-      <c r="A39" s="1" t="s">
+    <row r="38" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="39" spans="1:2" ht="15" customHeight="1">
+      <c r="A39" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="40" ht="15.0" customHeight="1">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="1:2" ht="15" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
@@ -870,7 +881,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" ht="15.0" customHeight="1">
+    <row r="41" spans="1:2" ht="15" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
@@ -878,7 +889,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" ht="15.0" customHeight="1">
+    <row r="42" spans="1:2" ht="15" customHeight="1">
       <c r="A42" s="1" t="s">
         <v>62</v>
       </c>
@@ -886,7 +897,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" ht="15.0" customHeight="1">
+    <row r="43" spans="1:2" ht="15" customHeight="1">
       <c r="A43" s="1" t="s">
         <v>63</v>
       </c>
@@ -894,13 +905,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" ht="12.75" customHeight="1"/>
-    <row r="45" ht="15.0" customHeight="1">
-      <c r="A45" s="1" t="s">
+    <row r="44" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="45" spans="1:2" ht="15" customHeight="1">
+      <c r="A45" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="46" ht="15.0" customHeight="1">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="1:2" ht="15" customHeight="1">
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
@@ -908,7 +920,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" ht="15.0" customHeight="1">
+    <row r="47" spans="1:2" ht="15" customHeight="1">
       <c r="A47" s="1" t="s">
         <v>68</v>
       </c>
@@ -916,7 +928,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="48" ht="15.0" customHeight="1">
+    <row r="48" spans="1:2" ht="15" customHeight="1">
       <c r="A48" s="1" t="s">
         <v>70</v>
       </c>
@@ -924,7 +936,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" ht="15.0" customHeight="1">
+    <row r="49" spans="1:2" ht="15" customHeight="1">
       <c r="A49" s="1" t="s">
         <v>72</v>
       </c>
@@ -932,13 +944,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" ht="12.75" customHeight="1"/>
-    <row r="51" ht="15.0" customHeight="1">
-      <c r="A51" s="1" t="s">
+    <row r="50" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="51" spans="1:2" ht="15" customHeight="1">
+      <c r="A51" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="52" ht="15.0" customHeight="1">
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="1:2" ht="15" customHeight="1">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -946,13 +959,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="53" ht="12.75" customHeight="1"/>
-    <row r="54" ht="15.0" customHeight="1">
-      <c r="A54" s="1" t="s">
+    <row r="53" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="54" spans="1:2" ht="15" customHeight="1">
+      <c r="A54" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="55" ht="15.0" customHeight="1">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>78</v>
       </c>
@@ -960,55 +974,56 @@
         <v>56</v>
       </c>
     </row>
-    <row r="56" ht="15.0" customHeight="1">
+    <row r="56" spans="1:2" ht="15" customHeight="1">
       <c r="B56" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="57" ht="15.0" customHeight="1">
+    <row r="57" spans="1:2" ht="15" customHeight="1">
       <c r="B57" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" ht="15.0" customHeight="1">
+    <row r="58" spans="1:2" ht="15" customHeight="1">
       <c r="B58" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" ht="15.0" customHeight="1">
+    <row r="59" spans="1:2" ht="15" customHeight="1">
       <c r="B59" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="60" ht="15.0" customHeight="1">
+    <row r="60" spans="1:2" ht="15" customHeight="1">
       <c r="B60" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="61" ht="15.0" customHeight="1">
+    <row r="61" spans="1:2" ht="15" customHeight="1">
       <c r="B61" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="62" ht="15.0" customHeight="1">
+    <row r="62" spans="1:2" ht="15" customHeight="1">
       <c r="B62" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" ht="15.0" customHeight="1">
+    <row r="63" spans="1:2" ht="15" customHeight="1">
       <c r="B63" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="64" ht="12.75" customHeight="1"/>
-    <row r="65" ht="12.75" customHeight="1"/>
-    <row r="66" ht="12.75" customHeight="1"/>
-    <row r="67" ht="15.0" customHeight="1">
-      <c r="A67" s="1" t="s">
+    <row r="64" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="65" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="66" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="67" spans="1:2" ht="15" customHeight="1">
+      <c r="A67" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" ht="15.0" customHeight="1">
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="1:2" ht="15" customHeight="1">
       <c r="A68" s="1" t="s">
         <v>22</v>
       </c>
@@ -1016,7 +1031,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" ht="15.0" customHeight="1">
+    <row r="69" spans="1:2" ht="15" customHeight="1">
       <c r="A69" s="1" t="s">
         <v>24</v>
       </c>
@@ -1024,7 +1039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" ht="15.0" customHeight="1">
+    <row r="70" spans="1:2" ht="15" customHeight="1">
       <c r="A70" s="1" t="s">
         <v>25</v>
       </c>
@@ -1032,7 +1047,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" ht="15.0" customHeight="1">
+    <row r="71" spans="1:2" ht="15" customHeight="1">
       <c r="A71" s="1" t="s">
         <v>27</v>
       </c>
@@ -1040,7 +1055,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" ht="15.0" customHeight="1">
+    <row r="72" spans="1:2" ht="15" customHeight="1">
       <c r="A72" s="1" t="s">
         <v>29</v>
       </c>
@@ -1048,7 +1063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" ht="15.0" customHeight="1">
+    <row r="73" spans="1:2" ht="15" customHeight="1">
       <c r="A73" s="1" t="s">
         <v>31</v>
       </c>
@@ -1056,7 +1071,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" ht="15.0" customHeight="1">
+    <row r="74" spans="1:2" ht="15" customHeight="1">
       <c r="A74" s="1" t="s">
         <v>33</v>
       </c>
@@ -1064,7 +1079,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" ht="15.0" customHeight="1">
+    <row r="75" spans="1:2" ht="15" customHeight="1">
       <c r="A75" s="1" t="s">
         <v>35</v>
       </c>
@@ -1072,7 +1087,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" ht="15.0" customHeight="1">
+    <row r="76" spans="1:2" ht="15" customHeight="1">
       <c r="A76" s="1" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1095,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" ht="15.0" customHeight="1">
+    <row r="77" spans="1:2" ht="15" customHeight="1">
       <c r="A77" s="1" t="s">
         <v>39</v>
       </c>
@@ -1088,7 +1103,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" ht="15.0" customHeight="1">
+    <row r="78" spans="1:2" ht="15" customHeight="1">
       <c r="A78" s="1" t="s">
         <v>41</v>
       </c>
@@ -1096,13 +1111,14 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" ht="12.75" customHeight="1"/>
-    <row r="80" ht="15.0" customHeight="1">
-      <c r="A80" s="1" t="s">
+    <row r="79" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="80" spans="1:2" ht="15" customHeight="1">
+      <c r="A80" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="81" ht="15.0" customHeight="1">
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="1:2" ht="15" customHeight="1">
       <c r="A81" s="1" t="s">
         <v>44</v>
       </c>
@@ -1110,7 +1126,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="82" ht="15.0" customHeight="1">
+    <row r="82" spans="1:2" ht="15" customHeight="1">
       <c r="A82" s="1" t="s">
         <v>46</v>
       </c>
@@ -1118,13 +1134,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" ht="12.75" customHeight="1"/>
-    <row r="84" ht="15.0" customHeight="1">
-      <c r="A84" s="1" t="s">
+    <row r="83" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="84" spans="1:2" ht="15" customHeight="1">
+      <c r="A84" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="85" ht="15.0" customHeight="1">
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" spans="1:2" ht="15" customHeight="1">
       <c r="A85" s="1" t="s">
         <v>49</v>
       </c>
@@ -1132,7 +1149,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" ht="15.0" customHeight="1">
+    <row r="86" spans="1:2" ht="15" customHeight="1">
       <c r="A86" s="1" t="s">
         <v>51</v>
       </c>
@@ -1140,13 +1157,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="87" ht="12.75" customHeight="1"/>
-    <row r="88" ht="15.0" customHeight="1">
-      <c r="A88" s="1" t="s">
+    <row r="87" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="88" spans="1:2" ht="15" customHeight="1">
+      <c r="A88" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="89" ht="15.0" customHeight="1">
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="1:2" ht="15" customHeight="1">
       <c r="A89" s="1" t="s">
         <v>44</v>
       </c>
@@ -1154,7 +1172,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="90" ht="15.0" customHeight="1">
+    <row r="90" spans="1:2" ht="15" customHeight="1">
       <c r="A90" s="1" t="s">
         <v>55</v>
       </c>
@@ -1162,13 +1180,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="91" ht="12.75" customHeight="1"/>
-    <row r="92" ht="15.0" customHeight="1">
-      <c r="A92" s="1" t="s">
+    <row r="91" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="92" spans="1:2" ht="15" customHeight="1">
+      <c r="A92" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="93" ht="15.0" customHeight="1">
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="1:2" ht="15" customHeight="1">
       <c r="A93" s="1" t="s">
         <v>58</v>
       </c>
@@ -1176,7 +1195,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" ht="15.0" customHeight="1">
+    <row r="94" spans="1:2" ht="15" customHeight="1">
       <c r="A94" s="1" t="s">
         <v>60</v>
       </c>
@@ -1184,7 +1203,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="95" ht="15.0" customHeight="1">
+    <row r="95" spans="1:2" ht="15" customHeight="1">
       <c r="A95" s="1" t="s">
         <v>62</v>
       </c>
@@ -1192,7 +1211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="96" ht="15.0" customHeight="1">
+    <row r="96" spans="1:2" ht="15" customHeight="1">
       <c r="A96" s="1" t="s">
         <v>63</v>
       </c>
@@ -1200,13 +1219,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" ht="12.75" customHeight="1"/>
-    <row r="98" ht="15.0" customHeight="1">
-      <c r="A98" s="1" t="s">
+    <row r="97" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="98" spans="1:2" ht="15" customHeight="1">
+      <c r="A98" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="99" ht="15.0" customHeight="1">
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="1:2" ht="15" customHeight="1">
       <c r="A99" s="1" t="s">
         <v>66</v>
       </c>
@@ -1214,7 +1234,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="100" ht="15.0" customHeight="1">
+    <row r="100" spans="1:2" ht="15" customHeight="1">
       <c r="A100" s="1" t="s">
         <v>68</v>
       </c>
@@ -1222,7 +1242,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="101" ht="15.0" customHeight="1">
+    <row r="101" spans="1:2" ht="15" customHeight="1">
       <c r="A101" s="1" t="s">
         <v>70</v>
       </c>
@@ -1230,7 +1250,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="102" ht="15.0" customHeight="1">
+    <row r="102" spans="1:2" ht="15" customHeight="1">
       <c r="A102" s="1" t="s">
         <v>72</v>
       </c>
@@ -1238,13 +1258,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" ht="12.75" customHeight="1"/>
-    <row r="104" ht="15.0" customHeight="1">
-      <c r="A104" s="1" t="s">
+    <row r="103" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="104" spans="1:2" ht="15" customHeight="1">
+      <c r="A104" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="105" ht="15.0" customHeight="1">
+      <c r="B104" s="5"/>
+    </row>
+    <row r="105" spans="1:2" ht="15" customHeight="1">
       <c r="A105" s="1" t="s">
         <v>75</v>
       </c>
@@ -1252,13 +1273,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" ht="12.75" customHeight="1"/>
-    <row r="107" ht="15.0" customHeight="1">
-      <c r="A107" s="1" t="s">
+    <row r="106" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="107" spans="1:2" ht="15" customHeight="1">
+      <c r="A107" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="108" ht="15.0" customHeight="1">
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="1:2" ht="15" customHeight="1">
       <c r="A108" s="2" t="s">
         <v>78</v>
       </c>
@@ -1266,18 +1288,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" ht="15.0" customHeight="1">
+    <row r="109" spans="1:2" ht="15" customHeight="1">
       <c r="B109" s="3"/>
     </row>
-    <row r="110" ht="15.0" customHeight="1">
+    <row r="110" spans="1:2" ht="15" customHeight="1">
       <c r="B110" s="3"/>
     </row>
-    <row r="111" ht="15.0" customHeight="1">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:2" ht="15" customHeight="1">
+      <c r="A111" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="112" ht="15.0" customHeight="1">
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="1:2" ht="15" customHeight="1">
       <c r="A112" s="1" t="s">
         <v>22</v>
       </c>
@@ -1285,7 +1308,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="113" ht="15.0" customHeight="1">
+    <row r="113" spans="1:2" ht="15" customHeight="1">
       <c r="A113" s="1" t="s">
         <v>24</v>
       </c>
@@ -1293,7 +1316,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" ht="15.0" customHeight="1">
+    <row r="114" spans="1:2" ht="15" customHeight="1">
       <c r="A114" s="1" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" ht="15.0" customHeight="1">
+    <row r="115" spans="1:2" ht="15" customHeight="1">
       <c r="A115" s="1" t="s">
         <v>27</v>
       </c>
@@ -1309,7 +1332,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" ht="15.0" customHeight="1">
+    <row r="116" spans="1:2" ht="15" customHeight="1">
       <c r="A116" s="1" t="s">
         <v>29</v>
       </c>
@@ -1317,7 +1340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" ht="15.0" customHeight="1">
+    <row r="117" spans="1:2" ht="15" customHeight="1">
       <c r="A117" s="1" t="s">
         <v>31</v>
       </c>
@@ -1325,7 +1348,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="118" ht="15.0" customHeight="1">
+    <row r="118" spans="1:2" ht="15" customHeight="1">
       <c r="A118" s="1" t="s">
         <v>33</v>
       </c>
@@ -1333,7 +1356,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" ht="15.0" customHeight="1">
+    <row r="119" spans="1:2" ht="15" customHeight="1">
       <c r="A119" s="1" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" ht="15.0" customHeight="1">
+    <row r="120" spans="1:2" ht="15" customHeight="1">
       <c r="A120" s="1" t="s">
         <v>37</v>
       </c>
@@ -1349,7 +1372,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" ht="15.0" customHeight="1">
+    <row r="121" spans="1:2" ht="15" customHeight="1">
       <c r="A121" s="1" t="s">
         <v>39</v>
       </c>
@@ -1357,7 +1380,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="122" ht="15.0" customHeight="1">
+    <row r="122" spans="1:2" ht="15" customHeight="1">
       <c r="A122" s="1" t="s">
         <v>41</v>
       </c>
@@ -1365,13 +1388,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="123" ht="12.75" customHeight="1"/>
-    <row r="124" ht="15.0" customHeight="1">
-      <c r="A124" s="1" t="s">
+    <row r="123" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="124" spans="1:2" ht="15" customHeight="1">
+      <c r="A124" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="125" ht="15.0" customHeight="1">
+      <c r="B124" s="5"/>
+    </row>
+    <row r="125" spans="1:2" ht="15" customHeight="1">
       <c r="A125" s="1" t="s">
         <v>44</v>
       </c>
@@ -1379,7 +1403,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="126" ht="15.0" customHeight="1">
+    <row r="126" spans="1:2" ht="15" customHeight="1">
       <c r="A126" s="1" t="s">
         <v>46</v>
       </c>
@@ -1387,13 +1411,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" ht="12.75" customHeight="1"/>
-    <row r="128" ht="15.0" customHeight="1">
-      <c r="A128" s="1" t="s">
+    <row r="127" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="128" spans="1:2" ht="15" customHeight="1">
+      <c r="A128" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="129" ht="15.0" customHeight="1">
+      <c r="B128" s="5"/>
+    </row>
+    <row r="129" spans="1:2" ht="15" customHeight="1">
       <c r="A129" s="1" t="s">
         <v>49</v>
       </c>
@@ -1401,7 +1426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="130" ht="15.0" customHeight="1">
+    <row r="130" spans="1:2" ht="15" customHeight="1">
       <c r="A130" s="1" t="s">
         <v>51</v>
       </c>
@@ -1409,13 +1434,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="131" ht="12.75" customHeight="1"/>
-    <row r="132" ht="15.0" customHeight="1">
-      <c r="A132" s="1" t="s">
+    <row r="131" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="132" spans="1:2" ht="15" customHeight="1">
+      <c r="A132" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="133" ht="15.0" customHeight="1">
+      <c r="B132" s="5"/>
+    </row>
+    <row r="133" spans="1:2" ht="15" customHeight="1">
       <c r="A133" s="1" t="s">
         <v>44</v>
       </c>
@@ -1423,7 +1449,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="134" ht="15.0" customHeight="1">
+    <row r="134" spans="1:2" ht="15" customHeight="1">
       <c r="A134" s="1" t="s">
         <v>55</v>
       </c>
@@ -1431,13 +1457,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="135" ht="12.75" customHeight="1"/>
-    <row r="136" ht="15.0" customHeight="1">
-      <c r="A136" s="1" t="s">
+    <row r="135" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="136" spans="1:2" ht="15" customHeight="1">
+      <c r="A136" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="137" ht="15.0" customHeight="1">
+      <c r="B136" s="5"/>
+    </row>
+    <row r="137" spans="1:2" ht="15" customHeight="1">
       <c r="A137" s="1" t="s">
         <v>58</v>
       </c>
@@ -1445,7 +1472,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="138" ht="15.0" customHeight="1">
+    <row r="138" spans="1:2" ht="15" customHeight="1">
       <c r="A138" s="1" t="s">
         <v>60</v>
       </c>
@@ -1453,7 +1480,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="139" ht="15.0" customHeight="1">
+    <row r="139" spans="1:2" ht="15" customHeight="1">
       <c r="A139" s="1" t="s">
         <v>62</v>
       </c>
@@ -1461,7 +1488,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="140" ht="15.0" customHeight="1">
+    <row r="140" spans="1:2" ht="15" customHeight="1">
       <c r="A140" s="1" t="s">
         <v>63</v>
       </c>
@@ -1469,13 +1496,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" ht="12.75" customHeight="1"/>
-    <row r="142" ht="15.0" customHeight="1">
-      <c r="A142" s="1" t="s">
+    <row r="141" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="142" spans="1:2" ht="15" customHeight="1">
+      <c r="A142" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="143" ht="15.0" customHeight="1">
+      <c r="B142" s="5"/>
+    </row>
+    <row r="143" spans="1:2" ht="15" customHeight="1">
       <c r="A143" s="1" t="s">
         <v>66</v>
       </c>
@@ -1483,7 +1511,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="144" ht="15.0" customHeight="1">
+    <row r="144" spans="1:2" ht="15" customHeight="1">
       <c r="A144" s="1" t="s">
         <v>68</v>
       </c>
@@ -1491,7 +1519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="145" ht="15.0" customHeight="1">
+    <row r="145" spans="1:2" ht="15" customHeight="1">
       <c r="A145" s="1" t="s">
         <v>70</v>
       </c>
@@ -1499,7 +1527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="146" ht="15.0" customHeight="1">
+    <row r="146" spans="1:2" ht="15" customHeight="1">
       <c r="A146" s="1" t="s">
         <v>72</v>
       </c>
@@ -1507,13 +1535,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" ht="12.75" customHeight="1"/>
-    <row r="148" ht="15.0" customHeight="1">
-      <c r="A148" s="1" t="s">
+    <row r="147" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="148" spans="1:2" ht="15" customHeight="1">
+      <c r="A148" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="149" ht="15.0" customHeight="1">
+      <c r="B148" s="5"/>
+    </row>
+    <row r="149" spans="1:2" ht="15" customHeight="1">
       <c r="A149" s="1" t="s">
         <v>75</v>
       </c>
@@ -1521,14 +1550,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="150" ht="12.75" customHeight="1"/>
-    <row r="151" ht="12.75" customHeight="1"/>
-    <row r="152" ht="15.0" customHeight="1">
-      <c r="A152" s="1" t="s">
+    <row r="150" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="151" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="152" spans="1:2" ht="15" customHeight="1">
+      <c r="A152" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="153" ht="15.0" customHeight="1">
+      <c r="B152" s="5"/>
+    </row>
+    <row r="153" spans="1:2" ht="15" customHeight="1">
       <c r="A153" s="1" t="s">
         <v>22</v>
       </c>
@@ -1536,7 +1566,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="154" ht="15.0" customHeight="1">
+    <row r="154" spans="1:2" ht="15" customHeight="1">
       <c r="A154" s="1" t="s">
         <v>24</v>
       </c>
@@ -1544,7 +1574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="155" ht="15.0" customHeight="1">
+    <row r="155" spans="1:2" ht="15" customHeight="1">
       <c r="A155" s="1" t="s">
         <v>25</v>
       </c>
@@ -1552,7 +1582,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="156" ht="15.0" customHeight="1">
+    <row r="156" spans="1:2" ht="15" customHeight="1">
       <c r="A156" s="1" t="s">
         <v>27</v>
       </c>
@@ -1560,7 +1590,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="157" ht="15.0" customHeight="1">
+    <row r="157" spans="1:2" ht="15" customHeight="1">
       <c r="A157" s="1" t="s">
         <v>29</v>
       </c>
@@ -1568,7 +1598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="158" ht="15.0" customHeight="1">
+    <row r="158" spans="1:2" ht="15" customHeight="1">
       <c r="A158" s="1" t="s">
         <v>31</v>
       </c>
@@ -1576,7 +1606,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="159" ht="15.0" customHeight="1">
+    <row r="159" spans="1:2" ht="15" customHeight="1">
       <c r="A159" s="1" t="s">
         <v>33</v>
       </c>
@@ -1584,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" ht="15.0" customHeight="1">
+    <row r="160" spans="1:2" ht="15" customHeight="1">
       <c r="A160" s="1" t="s">
         <v>35</v>
       </c>
@@ -1592,7 +1622,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" ht="15.0" customHeight="1">
+    <row r="161" spans="1:2" ht="15" customHeight="1">
       <c r="A161" s="1" t="s">
         <v>37</v>
       </c>
@@ -1600,7 +1630,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="162" ht="15.0" customHeight="1">
+    <row r="162" spans="1:2" ht="15" customHeight="1">
       <c r="A162" s="1" t="s">
         <v>39</v>
       </c>
@@ -1608,7 +1638,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" ht="15.0" customHeight="1">
+    <row r="163" spans="1:2" ht="15" customHeight="1">
       <c r="A163" s="1" t="s">
         <v>41</v>
       </c>
@@ -1616,13 +1646,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="164" ht="12.75" customHeight="1"/>
-    <row r="165" ht="15.0" customHeight="1">
-      <c r="A165" s="1" t="s">
+    <row r="164" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="165" spans="1:2" ht="15" customHeight="1">
+      <c r="A165" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="166" ht="15.0" customHeight="1">
+      <c r="B165" s="5"/>
+    </row>
+    <row r="166" spans="1:2" ht="15" customHeight="1">
       <c r="A166" s="1" t="s">
         <v>44</v>
       </c>
@@ -1630,7 +1661,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="167" ht="15.0" customHeight="1">
+    <row r="167" spans="1:2" ht="15" customHeight="1">
       <c r="A167" s="1" t="s">
         <v>46</v>
       </c>
@@ -1638,13 +1669,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="168" ht="12.75" customHeight="1"/>
-    <row r="169" ht="15.0" customHeight="1">
-      <c r="A169" s="1" t="s">
+    <row r="168" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="169" spans="1:2" ht="15" customHeight="1">
+      <c r="A169" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="170" ht="15.0" customHeight="1">
+      <c r="B169" s="5"/>
+    </row>
+    <row r="170" spans="1:2" ht="15" customHeight="1">
       <c r="A170" s="1" t="s">
         <v>49</v>
       </c>
@@ -1652,7 +1684,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="171" ht="15.0" customHeight="1">
+    <row r="171" spans="1:2" ht="15" customHeight="1">
       <c r="A171" s="1" t="s">
         <v>51</v>
       </c>
@@ -1660,13 +1692,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="172" ht="12.75" customHeight="1"/>
-    <row r="173" ht="15.0" customHeight="1">
-      <c r="A173" s="1" t="s">
+    <row r="172" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="173" spans="1:2" ht="15" customHeight="1">
+      <c r="A173" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="174" ht="15.0" customHeight="1">
+      <c r="B173" s="5"/>
+    </row>
+    <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="1" t="s">
         <v>44</v>
       </c>
@@ -1674,7 +1707,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="175" ht="15.0" customHeight="1">
+    <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="1" t="s">
         <v>55</v>
       </c>
@@ -1682,13 +1715,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="176" ht="12.75" customHeight="1"/>
-    <row r="177" ht="15.0" customHeight="1">
-      <c r="A177" s="1" t="s">
+    <row r="176" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="177" spans="1:2" ht="15" customHeight="1">
+      <c r="A177" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="178" ht="15.0" customHeight="1">
+      <c r="B177" s="5"/>
+    </row>
+    <row r="178" spans="1:2" ht="15" customHeight="1">
       <c r="A178" s="1" t="s">
         <v>58</v>
       </c>
@@ -1696,7 +1730,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="179" ht="15.0" customHeight="1">
+    <row r="179" spans="1:2" ht="15" customHeight="1">
       <c r="A179" s="1" t="s">
         <v>60</v>
       </c>
@@ -1704,7 +1738,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="180" ht="15.0" customHeight="1">
+    <row r="180" spans="1:2" ht="15" customHeight="1">
       <c r="A180" s="1" t="s">
         <v>96</v>
       </c>
@@ -1712,7 +1746,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="181" ht="15.0" customHeight="1">
+    <row r="181" spans="1:2" ht="15" customHeight="1">
       <c r="A181" s="1" t="s">
         <v>62</v>
       </c>
@@ -1720,7 +1754,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="182" ht="15.0" customHeight="1">
+    <row r="182" spans="1:2" ht="15" customHeight="1">
       <c r="A182" s="1" t="s">
         <v>63</v>
       </c>
@@ -1728,13 +1762,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="183" ht="12.75" customHeight="1"/>
-    <row r="184" ht="15.0" customHeight="1">
-      <c r="A184" s="1" t="s">
+    <row r="183" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="184" spans="1:2" ht="15" customHeight="1">
+      <c r="A184" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="185" ht="15.0" customHeight="1">
+      <c r="B184" s="5"/>
+    </row>
+    <row r="185" spans="1:2" ht="15" customHeight="1">
       <c r="A185" s="1" t="s">
         <v>66</v>
       </c>
@@ -1742,7 +1777,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="186" ht="15.0" customHeight="1">
+    <row r="186" spans="1:2" ht="15" customHeight="1">
       <c r="A186" s="1" t="s">
         <v>68</v>
       </c>
@@ -1750,7 +1785,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="187" ht="15.0" customHeight="1">
+    <row r="187" spans="1:2" ht="15" customHeight="1">
       <c r="A187" s="1" t="s">
         <v>70</v>
       </c>
@@ -1758,7 +1793,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="188" ht="15.0" customHeight="1">
+    <row r="188" spans="1:2" ht="15" customHeight="1">
       <c r="A188" s="1" t="s">
         <v>72</v>
       </c>
@@ -1766,13 +1801,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="189" ht="12.75" customHeight="1"/>
-    <row r="190" ht="15.0" customHeight="1">
-      <c r="A190" s="1" t="s">
+    <row r="189" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="190" spans="1:2" ht="15" customHeight="1">
+      <c r="A190" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="191" ht="15.0" customHeight="1">
+      <c r="B190" s="5"/>
+    </row>
+    <row r="191" spans="1:2" ht="15" customHeight="1">
       <c r="A191" s="1" t="s">
         <v>75</v>
       </c>
@@ -1780,14 +1816,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="192" ht="12.75" customHeight="1"/>
-    <row r="193" ht="12.75" customHeight="1"/>
-    <row r="194" ht="15.0" customHeight="1">
-      <c r="A194" s="1" t="s">
+    <row r="192" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="193" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="194" spans="1:2" ht="15" customHeight="1">
+      <c r="A194" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="195" ht="15.0" customHeight="1">
+      <c r="B194" s="5"/>
+    </row>
+    <row r="195" spans="1:2" ht="15" customHeight="1">
       <c r="A195" s="1" t="s">
         <v>22</v>
       </c>
@@ -1795,7 +1832,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="196" ht="15.0" customHeight="1">
+    <row r="196" spans="1:2" ht="15" customHeight="1">
       <c r="A196" s="1" t="s">
         <v>24</v>
       </c>
@@ -1803,7 +1840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" ht="15.0" customHeight="1">
+    <row r="197" spans="1:2" ht="15" customHeight="1">
       <c r="A197" s="1" t="s">
         <v>25</v>
       </c>
@@ -1811,7 +1848,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="198" ht="15.0" customHeight="1">
+    <row r="198" spans="1:2" ht="15" customHeight="1">
       <c r="A198" s="1" t="s">
         <v>27</v>
       </c>
@@ -1819,7 +1856,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="199" ht="15.0" customHeight="1">
+    <row r="199" spans="1:2" ht="15" customHeight="1">
       <c r="A199" s="1" t="s">
         <v>29</v>
       </c>
@@ -1827,7 +1864,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="200" ht="15.0" customHeight="1">
+    <row r="200" spans="1:2" ht="15" customHeight="1">
       <c r="A200" s="1" t="s">
         <v>31</v>
       </c>
@@ -1835,7 +1872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="201" ht="15.0" customHeight="1">
+    <row r="201" spans="1:2" ht="15" customHeight="1">
       <c r="A201" s="1" t="s">
         <v>33</v>
       </c>
@@ -1843,7 +1880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" ht="15.0" customHeight="1">
+    <row r="202" spans="1:2" ht="15" customHeight="1">
       <c r="A202" s="1" t="s">
         <v>35</v>
       </c>
@@ -1851,7 +1888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="203" ht="15.0" customHeight="1">
+    <row r="203" spans="1:2" ht="15" customHeight="1">
       <c r="A203" s="1" t="s">
         <v>37</v>
       </c>
@@ -1859,7 +1896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="204" ht="15.0" customHeight="1">
+    <row r="204" spans="1:2" ht="15" customHeight="1">
       <c r="A204" s="1" t="s">
         <v>39</v>
       </c>
@@ -1867,7 +1904,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="205" ht="15.0" customHeight="1">
+    <row r="205" spans="1:2" ht="15" customHeight="1">
       <c r="A205" s="1" t="s">
         <v>41</v>
       </c>
@@ -1875,13 +1912,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="206" ht="12.75" customHeight="1"/>
-    <row r="207" ht="15.0" customHeight="1">
-      <c r="A207" s="1" t="s">
+    <row r="206" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="207" spans="1:2" ht="15" customHeight="1">
+      <c r="A207" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="208" ht="15.0" customHeight="1">
+      <c r="B207" s="5"/>
+    </row>
+    <row r="208" spans="1:2" ht="15" customHeight="1">
       <c r="A208" s="1" t="s">
         <v>44</v>
       </c>
@@ -1889,7 +1927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="209" ht="15.0" customHeight="1">
+    <row r="209" spans="1:2" ht="15" customHeight="1">
       <c r="A209" s="1" t="s">
         <v>46</v>
       </c>
@@ -1897,13 +1935,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="210" ht="12.75" customHeight="1"/>
-    <row r="211" ht="15.0" customHeight="1">
-      <c r="A211" s="1" t="s">
+    <row r="210" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="211" spans="1:2" ht="15" customHeight="1">
+      <c r="A211" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="212" ht="15.0" customHeight="1">
+      <c r="B211" s="5"/>
+    </row>
+    <row r="212" spans="1:2" ht="15" customHeight="1">
       <c r="A212" s="1" t="s">
         <v>49</v>
       </c>
@@ -1911,7 +1950,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="213" ht="15.0" customHeight="1">
+    <row r="213" spans="1:2" ht="15" customHeight="1">
       <c r="A213" s="1" t="s">
         <v>51</v>
       </c>
@@ -1919,13 +1958,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="214" ht="12.75" customHeight="1"/>
-    <row r="215" ht="15.0" customHeight="1">
-      <c r="A215" s="1" t="s">
+    <row r="214" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="215" spans="1:2" ht="15" customHeight="1">
+      <c r="A215" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="216" ht="15.0" customHeight="1">
+      <c r="B215" s="5"/>
+    </row>
+    <row r="216" spans="1:2" ht="15" customHeight="1">
       <c r="A216" s="1" t="s">
         <v>44</v>
       </c>
@@ -1933,7 +1973,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="217" ht="15.0" customHeight="1">
+    <row r="217" spans="1:2" ht="15" customHeight="1">
       <c r="A217" s="1" t="s">
         <v>55</v>
       </c>
@@ -1941,13 +1981,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="218" ht="12.75" customHeight="1"/>
-    <row r="219" ht="15.0" customHeight="1">
-      <c r="A219" s="1" t="s">
+    <row r="218" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="219" spans="1:2" ht="15" customHeight="1">
+      <c r="A219" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="220" ht="15.0" customHeight="1">
+      <c r="B219" s="5"/>
+    </row>
+    <row r="220" spans="1:2" ht="15" customHeight="1">
       <c r="A220" s="1" t="s">
         <v>58</v>
       </c>
@@ -1955,7 +1996,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="221" ht="15.0" customHeight="1">
+    <row r="221" spans="1:2" ht="15" customHeight="1">
       <c r="A221" s="1" t="s">
         <v>60</v>
       </c>
@@ -1963,7 +2004,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="222" ht="15.0" customHeight="1">
+    <row r="222" spans="1:2" ht="15" customHeight="1">
       <c r="A222" s="1" t="s">
         <v>96</v>
       </c>
@@ -1971,7 +2012,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="223" ht="15.0" customHeight="1">
+    <row r="223" spans="1:2" ht="15" customHeight="1">
       <c r="A223" s="1" t="s">
         <v>62</v>
       </c>
@@ -1979,7 +2020,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="224" ht="15.0" customHeight="1">
+    <row r="224" spans="1:2" ht="15" customHeight="1">
       <c r="A224" s="1" t="s">
         <v>63</v>
       </c>
@@ -1987,13 +2028,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="225" ht="12.75" customHeight="1"/>
-    <row r="226" ht="15.0" customHeight="1">
-      <c r="A226" s="1" t="s">
+    <row r="225" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="226" spans="1:2" ht="15" customHeight="1">
+      <c r="A226" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="227" ht="15.0" customHeight="1">
+      <c r="B226" s="5"/>
+    </row>
+    <row r="227" spans="1:2" ht="15" customHeight="1">
       <c r="A227" s="1" t="s">
         <v>66</v>
       </c>
@@ -2001,7 +2043,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="228" ht="15.0" customHeight="1">
+    <row r="228" spans="1:2" ht="15" customHeight="1">
       <c r="A228" s="1" t="s">
         <v>68</v>
       </c>
@@ -2009,7 +2051,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="229" ht="15.0" customHeight="1">
+    <row r="229" spans="1:2" ht="15" customHeight="1">
       <c r="A229" s="1" t="s">
         <v>70</v>
       </c>
@@ -2017,7 +2059,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="230" ht="15.0" customHeight="1">
+    <row r="230" spans="1:2" ht="15" customHeight="1">
       <c r="A230" s="1" t="s">
         <v>72</v>
       </c>
@@ -2025,13 +2067,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="231" ht="12.75" customHeight="1"/>
-    <row r="232" ht="15.0" customHeight="1">
-      <c r="A232" s="1" t="s">
+    <row r="231" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="232" spans="1:2" ht="15" customHeight="1">
+      <c r="A232" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="233" ht="15.0" customHeight="1">
+      <c r="B232" s="5"/>
+    </row>
+    <row r="233" spans="1:2" ht="15" customHeight="1">
       <c r="A233" s="1" t="s">
         <v>75</v>
       </c>
@@ -2039,14 +2082,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="234" ht="12.75" customHeight="1"/>
-    <row r="235" ht="12.75" customHeight="1"/>
-    <row r="236" ht="15.0" customHeight="1">
-      <c r="A236" s="1" t="s">
+    <row r="234" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="235" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="236" spans="1:2" ht="15" customHeight="1">
+      <c r="A236" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="237" ht="15.0" customHeight="1">
+      <c r="B236" s="5"/>
+    </row>
+    <row r="237" spans="1:2" ht="15" customHeight="1">
       <c r="A237" s="1" t="s">
         <v>22</v>
       </c>
@@ -2054,7 +2098,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="238" ht="15.0" customHeight="1">
+    <row r="238" spans="1:2" ht="15" customHeight="1">
       <c r="A238" s="1" t="s">
         <v>24</v>
       </c>
@@ -2062,7 +2106,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" ht="15.0" customHeight="1">
+    <row r="239" spans="1:2" ht="15" customHeight="1">
       <c r="A239" s="1" t="s">
         <v>25</v>
       </c>
@@ -2070,7 +2114,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="240" ht="15.0" customHeight="1">
+    <row r="240" spans="1:2" ht="15" customHeight="1">
       <c r="A240" s="1" t="s">
         <v>27</v>
       </c>
@@ -2078,7 +2122,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="241" ht="15.0" customHeight="1">
+    <row r="241" spans="1:2" ht="15" customHeight="1">
       <c r="A241" s="1" t="s">
         <v>29</v>
       </c>
@@ -2086,7 +2130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="242" ht="15.0" customHeight="1">
+    <row r="242" spans="1:2" ht="15" customHeight="1">
       <c r="A242" s="1" t="s">
         <v>31</v>
       </c>
@@ -2094,7 +2138,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="243" ht="15.0" customHeight="1">
+    <row r="243" spans="1:2" ht="15" customHeight="1">
       <c r="A243" s="1" t="s">
         <v>33</v>
       </c>
@@ -2102,7 +2146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="244" ht="15.0" customHeight="1">
+    <row r="244" spans="1:2" ht="15" customHeight="1">
       <c r="A244" s="1" t="s">
         <v>35</v>
       </c>
@@ -2110,7 +2154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="245" ht="15.0" customHeight="1">
+    <row r="245" spans="1:2" ht="15" customHeight="1">
       <c r="A245" s="1" t="s">
         <v>37</v>
       </c>
@@ -2118,7 +2162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="246" ht="15.0" customHeight="1">
+    <row r="246" spans="1:2" ht="15" customHeight="1">
       <c r="A246" s="1" t="s">
         <v>39</v>
       </c>
@@ -2126,7 +2170,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="247" ht="15.0" customHeight="1">
+    <row r="247" spans="1:2" ht="15" customHeight="1">
       <c r="A247" s="1" t="s">
         <v>41</v>
       </c>
@@ -2134,13 +2178,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="248" ht="12.75" customHeight="1"/>
-    <row r="249" ht="15.0" customHeight="1">
-      <c r="A249" s="1" t="s">
+    <row r="248" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="249" spans="1:2" ht="15" customHeight="1">
+      <c r="A249" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="250" ht="15.0" customHeight="1">
+      <c r="B249" s="5"/>
+    </row>
+    <row r="250" spans="1:2" ht="15" customHeight="1">
       <c r="A250" s="1" t="s">
         <v>44</v>
       </c>
@@ -2148,7 +2193,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="251" ht="15.0" customHeight="1">
+    <row r="251" spans="1:2" ht="15" customHeight="1">
       <c r="A251" s="1" t="s">
         <v>46</v>
       </c>
@@ -2156,13 +2201,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="252" ht="12.75" customHeight="1"/>
-    <row r="253" ht="15.0" customHeight="1">
-      <c r="A253" s="1" t="s">
+    <row r="252" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="253" spans="1:2" ht="15" customHeight="1">
+      <c r="A253" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="254" ht="15.0" customHeight="1">
+      <c r="B253" s="5"/>
+    </row>
+    <row r="254" spans="1:2" ht="15" customHeight="1">
       <c r="A254" s="1" t="s">
         <v>49</v>
       </c>
@@ -2170,7 +2216,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="255" ht="15.0" customHeight="1">
+    <row r="255" spans="1:2" ht="15" customHeight="1">
       <c r="A255" s="1" t="s">
         <v>51</v>
       </c>
@@ -2178,13 +2224,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="256" ht="12.75" customHeight="1"/>
-    <row r="257" ht="15.0" customHeight="1">
-      <c r="A257" s="1" t="s">
+    <row r="256" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="257" spans="1:2" ht="15" customHeight="1">
+      <c r="A257" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="258" ht="15.0" customHeight="1">
+      <c r="B257" s="5"/>
+    </row>
+    <row r="258" spans="1:2" ht="15" customHeight="1">
       <c r="A258" s="1" t="s">
         <v>44</v>
       </c>
@@ -2192,7 +2239,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="259" ht="15.0" customHeight="1">
+    <row r="259" spans="1:2" ht="15" customHeight="1">
       <c r="A259" s="1" t="s">
         <v>55</v>
       </c>
@@ -2200,13 +2247,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="260" ht="12.75" customHeight="1"/>
-    <row r="261" ht="15.0" customHeight="1">
-      <c r="A261" s="1" t="s">
+    <row r="260" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="261" spans="1:2" ht="15" customHeight="1">
+      <c r="A261" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="262" ht="15.0" customHeight="1">
+      <c r="B261" s="5"/>
+    </row>
+    <row r="262" spans="1:2" ht="15" customHeight="1">
       <c r="A262" s="1" t="s">
         <v>58</v>
       </c>
@@ -2214,7 +2262,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="263" ht="15.0" customHeight="1">
+    <row r="263" spans="1:2" ht="15" customHeight="1">
       <c r="A263" s="1" t="s">
         <v>60</v>
       </c>
@@ -2222,7 +2270,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="264" ht="15.0" customHeight="1">
+    <row r="264" spans="1:2" ht="15" customHeight="1">
       <c r="A264" s="1" t="s">
         <v>96</v>
       </c>
@@ -2230,7 +2278,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="265" ht="15.0" customHeight="1">
+    <row r="265" spans="1:2" ht="15" customHeight="1">
       <c r="A265" s="1" t="s">
         <v>62</v>
       </c>
@@ -2238,7 +2286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="266" ht="15.0" customHeight="1">
+    <row r="266" spans="1:2" ht="15" customHeight="1">
       <c r="A266" s="1" t="s">
         <v>63</v>
       </c>
@@ -2246,13 +2294,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="267" ht="12.75" customHeight="1"/>
-    <row r="268" ht="15.0" customHeight="1">
-      <c r="A268" s="1" t="s">
+    <row r="267" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="268" spans="1:2" ht="15" customHeight="1">
+      <c r="A268" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="269" ht="15.0" customHeight="1">
+      <c r="B268" s="5"/>
+    </row>
+    <row r="269" spans="1:2" ht="15" customHeight="1">
       <c r="A269" s="1" t="s">
         <v>66</v>
       </c>
@@ -2260,7 +2309,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="270" ht="15.0" customHeight="1">
+    <row r="270" spans="1:2" ht="15" customHeight="1">
       <c r="A270" s="1" t="s">
         <v>68</v>
       </c>
@@ -2268,7 +2317,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="271" ht="15.0" customHeight="1">
+    <row r="271" spans="1:2" ht="15" customHeight="1">
       <c r="A271" s="1" t="s">
         <v>70</v>
       </c>
@@ -2276,7 +2325,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="272" ht="15.0" customHeight="1">
+    <row r="272" spans="1:2" ht="15" customHeight="1">
       <c r="A272" s="1" t="s">
         <v>72</v>
       </c>
@@ -2284,13 +2333,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="273" ht="12.75" customHeight="1"/>
-    <row r="274" ht="15.0" customHeight="1">
-      <c r="A274" s="1" t="s">
+    <row r="273" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="274" spans="1:2" ht="15" customHeight="1">
+      <c r="A274" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="275" ht="15.0" customHeight="1">
+      <c r="B274" s="5"/>
+    </row>
+    <row r="275" spans="1:2" ht="15" customHeight="1">
       <c r="A275" s="1" t="s">
         <v>75</v>
       </c>
@@ -2298,14 +2348,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="276" ht="12.75" customHeight="1"/>
-    <row r="277" ht="12.75" customHeight="1"/>
-    <row r="278" ht="15.0" customHeight="1">
-      <c r="A278" s="1" t="s">
+    <row r="276" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="277" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="278" spans="1:2" ht="15" customHeight="1">
+      <c r="A278" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="279" ht="15.0" customHeight="1">
+      <c r="B278" s="5"/>
+    </row>
+    <row r="279" spans="1:2" ht="15" customHeight="1">
       <c r="A279" s="1" t="s">
         <v>22</v>
       </c>
@@ -2313,7 +2364,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="280" ht="15.0" customHeight="1">
+    <row r="280" spans="1:2" ht="15" customHeight="1">
       <c r="A280" s="1" t="s">
         <v>24</v>
       </c>
@@ -2321,7 +2372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="281" ht="15.0" customHeight="1">
+    <row r="281" spans="1:2" ht="15" customHeight="1">
       <c r="A281" s="1" t="s">
         <v>25</v>
       </c>
@@ -2329,7 +2380,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="282" ht="15.0" customHeight="1">
+    <row r="282" spans="1:2" ht="15" customHeight="1">
       <c r="A282" s="1" t="s">
         <v>27</v>
       </c>
@@ -2337,7 +2388,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="283" ht="15.0" customHeight="1">
+    <row r="283" spans="1:2" ht="15" customHeight="1">
       <c r="A283" s="1" t="s">
         <v>29</v>
       </c>
@@ -2345,7 +2396,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="284" ht="15.0" customHeight="1">
+    <row r="284" spans="1:2" ht="15" customHeight="1">
       <c r="A284" s="1" t="s">
         <v>31</v>
       </c>
@@ -2353,7 +2404,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="285" ht="15.0" customHeight="1">
+    <row r="285" spans="1:2" ht="15" customHeight="1">
       <c r="A285" s="1" t="s">
         <v>33</v>
       </c>
@@ -2361,7 +2412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="286" ht="15.0" customHeight="1">
+    <row r="286" spans="1:2" ht="15" customHeight="1">
       <c r="A286" s="1" t="s">
         <v>35</v>
       </c>
@@ -2369,7 +2420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="287" ht="15.0" customHeight="1">
+    <row r="287" spans="1:2" ht="15" customHeight="1">
       <c r="A287" s="1" t="s">
         <v>37</v>
       </c>
@@ -2377,7 +2428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="288" ht="15.0" customHeight="1">
+    <row r="288" spans="1:2" ht="15" customHeight="1">
       <c r="A288" s="1" t="s">
         <v>39</v>
       </c>
@@ -2385,7 +2436,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="289" ht="15.0" customHeight="1">
+    <row r="289" spans="1:2" ht="15" customHeight="1">
       <c r="A289" s="1" t="s">
         <v>41</v>
       </c>
@@ -2393,13 +2444,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="290" ht="12.75" customHeight="1"/>
-    <row r="291" ht="15.0" customHeight="1">
-      <c r="A291" s="1" t="s">
+    <row r="290" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="291" spans="1:2" ht="15" customHeight="1">
+      <c r="A291" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="292" ht="15.0" customHeight="1">
+      <c r="B291" s="5"/>
+    </row>
+    <row r="292" spans="1:2" ht="15" customHeight="1">
       <c r="A292" s="1" t="s">
         <v>44</v>
       </c>
@@ -2407,7 +2459,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="293" ht="15.0" customHeight="1">
+    <row r="293" spans="1:2" ht="15" customHeight="1">
       <c r="A293" s="1" t="s">
         <v>46</v>
       </c>
@@ -2415,13 +2467,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="294" ht="12.75" customHeight="1"/>
-    <row r="295" ht="15.0" customHeight="1">
-      <c r="A295" s="1" t="s">
+    <row r="294" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="295" spans="1:2" ht="15" customHeight="1">
+      <c r="A295" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="296" ht="15.0" customHeight="1">
+      <c r="B295" s="5"/>
+    </row>
+    <row r="296" spans="1:2" ht="15" customHeight="1">
       <c r="A296" s="1" t="s">
         <v>49</v>
       </c>
@@ -2429,7 +2482,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="297" ht="15.0" customHeight="1">
+    <row r="297" spans="1:2" ht="15" customHeight="1">
       <c r="A297" s="1" t="s">
         <v>51</v>
       </c>
@@ -2437,13 +2490,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="298" ht="12.75" customHeight="1"/>
-    <row r="299" ht="15.0" customHeight="1">
-      <c r="A299" s="1" t="s">
+    <row r="298" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="299" spans="1:2" ht="15" customHeight="1">
+      <c r="A299" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="300" ht="15.0" customHeight="1">
+      <c r="B299" s="5"/>
+    </row>
+    <row r="300" spans="1:2" ht="15" customHeight="1">
       <c r="A300" s="1" t="s">
         <v>44</v>
       </c>
@@ -2451,7 +2505,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="301" ht="15.0" customHeight="1">
+    <row r="301" spans="1:2" ht="15" customHeight="1">
       <c r="A301" s="1" t="s">
         <v>55</v>
       </c>
@@ -2459,13 +2513,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="302" ht="12.75" customHeight="1"/>
-    <row r="303" ht="15.0" customHeight="1">
-      <c r="A303" s="1" t="s">
+    <row r="302" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="303" spans="1:2" ht="15" customHeight="1">
+      <c r="A303" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="304" ht="15.0" customHeight="1">
+      <c r="B303" s="5"/>
+    </row>
+    <row r="304" spans="1:2" ht="15" customHeight="1">
       <c r="A304" s="1" t="s">
         <v>58</v>
       </c>
@@ -2473,7 +2528,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="305" ht="15.0" customHeight="1">
+    <row r="305" spans="1:2" ht="15" customHeight="1">
       <c r="A305" s="1" t="s">
         <v>60</v>
       </c>
@@ -2481,7 +2536,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="306" ht="15.0" customHeight="1">
+    <row r="306" spans="1:2" ht="15" customHeight="1">
       <c r="A306" s="1" t="s">
         <v>96</v>
       </c>
@@ -2489,7 +2544,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="307" ht="15.0" customHeight="1">
+    <row r="307" spans="1:2" ht="15" customHeight="1">
       <c r="A307" s="1" t="s">
         <v>62</v>
       </c>
@@ -2497,7 +2552,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="308" ht="15.0" customHeight="1">
+    <row r="308" spans="1:2" ht="15" customHeight="1">
       <c r="A308" s="1" t="s">
         <v>63</v>
       </c>
@@ -2505,13 +2560,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="309" ht="12.75" customHeight="1"/>
-    <row r="310" ht="15.0" customHeight="1">
-      <c r="A310" s="1" t="s">
+    <row r="309" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="310" spans="1:2" ht="15" customHeight="1">
+      <c r="A310" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="311" ht="15.0" customHeight="1">
+      <c r="B310" s="5"/>
+    </row>
+    <row r="311" spans="1:2" ht="15" customHeight="1">
       <c r="A311" s="1" t="s">
         <v>66</v>
       </c>
@@ -2519,7 +2575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="312" ht="15.0" customHeight="1">
+    <row r="312" spans="1:2" ht="15" customHeight="1">
       <c r="A312" s="1" t="s">
         <v>68</v>
       </c>
@@ -2527,7 +2583,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="313" ht="15.0" customHeight="1">
+    <row r="313" spans="1:2" ht="15" customHeight="1">
       <c r="A313" s="1" t="s">
         <v>70</v>
       </c>
@@ -2535,7 +2591,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="314" ht="15.0" customHeight="1">
+    <row r="314" spans="1:2" ht="15" customHeight="1">
       <c r="A314" s="1" t="s">
         <v>72</v>
       </c>
@@ -2543,13 +2599,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="315" ht="12.75" customHeight="1"/>
-    <row r="316" ht="15.0" customHeight="1">
-      <c r="A316" s="1" t="s">
+    <row r="315" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="316" spans="1:2" ht="15" customHeight="1">
+      <c r="A316" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="317" ht="15.0" customHeight="1">
+      <c r="B316" s="5"/>
+    </row>
+    <row r="317" spans="1:2" ht="15" customHeight="1">
       <c r="A317" s="1" t="s">
         <v>75</v>
       </c>
@@ -2557,14 +2614,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="318" ht="12.75" customHeight="1"/>
-    <row r="319" ht="12.75" customHeight="1"/>
-    <row r="320" ht="15.0" customHeight="1">
-      <c r="A320" s="1" t="s">
+    <row r="318" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="319" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="320" spans="1:2" ht="15" customHeight="1">
+      <c r="A320" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="321" ht="15.0" customHeight="1">
+      <c r="B320" s="5"/>
+    </row>
+    <row r="321" spans="1:2" ht="15" customHeight="1">
       <c r="A321" s="1" t="s">
         <v>22</v>
       </c>
@@ -2572,7 +2630,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="322" ht="15.0" customHeight="1">
+    <row r="322" spans="1:2" ht="15" customHeight="1">
       <c r="A322" s="1" t="s">
         <v>24</v>
       </c>
@@ -2580,7 +2638,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="323" ht="15.0" customHeight="1">
+    <row r="323" spans="1:2" ht="15" customHeight="1">
       <c r="A323" s="1" t="s">
         <v>25</v>
       </c>
@@ -2588,7 +2646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="324" ht="15.0" customHeight="1">
+    <row r="324" spans="1:2" ht="15" customHeight="1">
       <c r="A324" s="1" t="s">
         <v>27</v>
       </c>
@@ -2596,7 +2654,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="325" ht="15.0" customHeight="1">
+    <row r="325" spans="1:2" ht="15" customHeight="1">
       <c r="A325" s="1" t="s">
         <v>29</v>
       </c>
@@ -2604,7 +2662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="326" ht="15.0" customHeight="1">
+    <row r="326" spans="1:2" ht="15" customHeight="1">
       <c r="A326" s="1" t="s">
         <v>31</v>
       </c>
@@ -2612,7 +2670,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="327" ht="15.0" customHeight="1">
+    <row r="327" spans="1:2" ht="15" customHeight="1">
       <c r="A327" s="1" t="s">
         <v>33</v>
       </c>
@@ -2620,7 +2678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" ht="15.0" customHeight="1">
+    <row r="328" spans="1:2" ht="15" customHeight="1">
       <c r="A328" s="1" t="s">
         <v>35</v>
       </c>
@@ -2628,7 +2686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="329" ht="15.0" customHeight="1">
+    <row r="329" spans="1:2" ht="15" customHeight="1">
       <c r="A329" s="1" t="s">
         <v>37</v>
       </c>
@@ -2636,7 +2694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="330" ht="15.0" customHeight="1">
+    <row r="330" spans="1:2" ht="15" customHeight="1">
       <c r="A330" s="1" t="s">
         <v>39</v>
       </c>
@@ -2644,7 +2702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="331" ht="15.0" customHeight="1">
+    <row r="331" spans="1:2" ht="15" customHeight="1">
       <c r="A331" s="1" t="s">
         <v>41</v>
       </c>
@@ -2652,13 +2710,14 @@
         <v>93</v>
       </c>
     </row>
-    <row r="332" ht="12.75" customHeight="1"/>
-    <row r="333" ht="15.0" customHeight="1">
-      <c r="A333" s="1" t="s">
+    <row r="332" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="333" spans="1:2" ht="15" customHeight="1">
+      <c r="A333" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="334" ht="15.0" customHeight="1">
+      <c r="B333" s="5"/>
+    </row>
+    <row r="334" spans="1:2" ht="15" customHeight="1">
       <c r="A334" s="1" t="s">
         <v>44</v>
       </c>
@@ -2666,7 +2725,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="335" ht="15.0" customHeight="1">
+    <row r="335" spans="1:2" ht="15" customHeight="1">
       <c r="A335" s="1" t="s">
         <v>46</v>
       </c>
@@ -2674,13 +2733,14 @@
         <v>47</v>
       </c>
     </row>
-    <row r="336" ht="12.75" customHeight="1"/>
-    <row r="337" ht="15.0" customHeight="1">
-      <c r="A337" s="1" t="s">
+    <row r="336" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="337" spans="1:2" ht="15" customHeight="1">
+      <c r="A337" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="338" ht="15.0" customHeight="1">
+      <c r="B337" s="5"/>
+    </row>
+    <row r="338" spans="1:2" ht="15" customHeight="1">
       <c r="A338" s="1" t="s">
         <v>49</v>
       </c>
@@ -2688,7 +2748,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="339" ht="15.0" customHeight="1">
+    <row r="339" spans="1:2" ht="15" customHeight="1">
       <c r="A339" s="1" t="s">
         <v>51</v>
       </c>
@@ -2696,13 +2756,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="340" ht="12.75" customHeight="1"/>
-    <row r="341" ht="15.0" customHeight="1">
-      <c r="A341" s="1" t="s">
+    <row r="340" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="341" spans="1:2" ht="15" customHeight="1">
+      <c r="A341" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="342" ht="15.0" customHeight="1">
+      <c r="B341" s="5"/>
+    </row>
+    <row r="342" spans="1:2" ht="15" customHeight="1">
       <c r="A342" s="1" t="s">
         <v>44</v>
       </c>
@@ -2710,7 +2771,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="343" ht="15.0" customHeight="1">
+    <row r="343" spans="1:2" ht="15" customHeight="1">
       <c r="A343" s="1" t="s">
         <v>55</v>
       </c>
@@ -2718,13 +2779,14 @@
         <v>56</v>
       </c>
     </row>
-    <row r="344" ht="12.75" customHeight="1"/>
-    <row r="345" ht="15.0" customHeight="1">
-      <c r="A345" s="1" t="s">
+    <row r="344" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="345" spans="1:2" ht="15" customHeight="1">
+      <c r="A345" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="346" ht="15.0" customHeight="1">
+      <c r="B345" s="5"/>
+    </row>
+    <row r="346" spans="1:2" ht="15" customHeight="1">
       <c r="A346" s="1" t="s">
         <v>58</v>
       </c>
@@ -2732,7 +2794,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="347" ht="15.0" customHeight="1">
+    <row r="347" spans="1:2" ht="15" customHeight="1">
       <c r="A347" s="1" t="s">
         <v>60</v>
       </c>
@@ -2740,7 +2802,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="348" ht="15.0" customHeight="1">
+    <row r="348" spans="1:2" ht="15" customHeight="1">
       <c r="A348" s="1" t="s">
         <v>96</v>
       </c>
@@ -2748,7 +2810,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="349" ht="15.0" customHeight="1">
+    <row r="349" spans="1:2" ht="15" customHeight="1">
       <c r="A349" s="1" t="s">
         <v>62</v>
       </c>
@@ -2756,7 +2818,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="350" ht="15.0" customHeight="1">
+    <row r="350" spans="1:2" ht="15" customHeight="1">
       <c r="A350" s="1" t="s">
         <v>63</v>
       </c>
@@ -2764,13 +2826,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="351" ht="12.75" customHeight="1"/>
-    <row r="352" ht="15.0" customHeight="1">
-      <c r="A352" s="1" t="s">
+    <row r="351" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="352" spans="1:2" ht="15" customHeight="1">
+      <c r="A352" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="353" ht="15.0" customHeight="1">
+      <c r="B352" s="5"/>
+    </row>
+    <row r="353" spans="1:2" ht="15" customHeight="1">
       <c r="A353" s="1" t="s">
         <v>66</v>
       </c>
@@ -2778,7 +2841,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="354" ht="15.0" customHeight="1">
+    <row r="354" spans="1:2" ht="15" customHeight="1">
       <c r="A354" s="1" t="s">
         <v>68</v>
       </c>
@@ -2786,7 +2849,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="355" ht="15.0" customHeight="1">
+    <row r="355" spans="1:2" ht="15" customHeight="1">
       <c r="A355" s="1" t="s">
         <v>70</v>
       </c>
@@ -2794,7 +2857,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="356" ht="15.0" customHeight="1">
+    <row r="356" spans="1:2" ht="15" customHeight="1">
       <c r="A356" s="1" t="s">
         <v>72</v>
       </c>
@@ -2802,13 +2865,14 @@
         <v>90</v>
       </c>
     </row>
-    <row r="357" ht="12.75" customHeight="1"/>
-    <row r="358" ht="15.0" customHeight="1">
-      <c r="A358" s="1" t="s">
+    <row r="357" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="358" spans="1:2" ht="15" customHeight="1">
+      <c r="A358" s="4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="359" ht="15.0" customHeight="1">
+      <c r="B358" s="5"/>
+    </row>
+    <row r="359" spans="1:2" ht="15" customHeight="1">
       <c r="A359" s="1" t="s">
         <v>75</v>
       </c>
@@ -2816,15 +2880,15 @@
         <v>76</v>
       </c>
     </row>
-    <row r="360" ht="12.75" customHeight="1"/>
-    <row r="361" ht="12.75" customHeight="1"/>
-    <row r="362" ht="12.75" customHeight="1"/>
-    <row r="363" ht="12.75" customHeight="1"/>
-    <row r="364" ht="12.75" customHeight="1"/>
-    <row r="365" ht="12.75" customHeight="1"/>
-    <row r="366" ht="12.75" customHeight="1"/>
-    <row r="367" ht="12.75" customHeight="1"/>
-    <row r="368" ht="12.75" customHeight="1"/>
+    <row r="360" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="361" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="362" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="363" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="364" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="365" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="366" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="367" spans="1:2" ht="12.75" customHeight="1"/>
+    <row r="368" spans="1:2" ht="12.75" customHeight="1"/>
     <row r="369" ht="12.75" customHeight="1"/>
     <row r="370" ht="12.75" customHeight="1"/>
     <row r="371" ht="12.75" customHeight="1"/>
@@ -3450,6 +3514,55 @@
     <row r="991" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="A278:B278"/>
+    <mergeCell ref="A291:B291"/>
+    <mergeCell ref="A295:B295"/>
+    <mergeCell ref="A299:B299"/>
+    <mergeCell ref="A253:B253"/>
+    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="A261:B261"/>
+    <mergeCell ref="A268:B268"/>
+    <mergeCell ref="A274:B274"/>
+    <mergeCell ref="A219:B219"/>
+    <mergeCell ref="A226:B226"/>
+    <mergeCell ref="A232:B232"/>
+    <mergeCell ref="A236:B236"/>
+    <mergeCell ref="A249:B249"/>
+    <mergeCell ref="A190:B190"/>
+    <mergeCell ref="A194:B194"/>
+    <mergeCell ref="A207:B207"/>
+    <mergeCell ref="A211:B211"/>
+    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="A177:B177"/>
+    <mergeCell ref="A184:B184"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="A142:B142"/>
+    <mergeCell ref="A148:B148"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="A345:B345"/>
     <mergeCell ref="A352:B352"/>
     <mergeCell ref="A358:B358"/>
@@ -3460,443 +3573,779 @@
     <mergeCell ref="A333:B333"/>
     <mergeCell ref="A337:B337"/>
     <mergeCell ref="A341:B341"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="A128:B128"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A136:B136"/>
-    <mergeCell ref="A142:B142"/>
-    <mergeCell ref="A148:B148"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="A177:B177"/>
-    <mergeCell ref="A184:B184"/>
-    <mergeCell ref="A190:B190"/>
-    <mergeCell ref="A194:B194"/>
-    <mergeCell ref="A207:B207"/>
-    <mergeCell ref="A211:B211"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="A219:B219"/>
-    <mergeCell ref="A226:B226"/>
-    <mergeCell ref="A232:B232"/>
-    <mergeCell ref="A236:B236"/>
-    <mergeCell ref="A249:B249"/>
-    <mergeCell ref="A253:B253"/>
-    <mergeCell ref="A257:B257"/>
-    <mergeCell ref="A261:B261"/>
-    <mergeCell ref="A268:B268"/>
-    <mergeCell ref="A274:B274"/>
-    <mergeCell ref="A278:B278"/>
-    <mergeCell ref="A291:B291"/>
-    <mergeCell ref="A295:B295"/>
-    <mergeCell ref="A299:B299"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L1" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="M1" s="3">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B2" s="3">
-        <v>7983909.0</v>
+        <v>7983909</v>
       </c>
       <c r="C2" s="3">
-        <v>7564875.0</v>
+        <v>7564875</v>
       </c>
       <c r="D2" s="3">
-        <v>4650965.0</v>
+        <v>4650965</v>
       </c>
       <c r="E2" s="3">
-        <v>4291172.0</v>
+        <v>4291172</v>
       </c>
       <c r="F2" s="3">
-        <v>4430788.0</v>
+        <v>4430788</v>
       </c>
       <c r="G2" s="3">
-        <v>3019.0</v>
+        <v>3019</v>
       </c>
       <c r="H2" s="3">
-        <v>3710.0</v>
+        <v>3710</v>
       </c>
       <c r="I2" s="3">
-        <v>3060.0</v>
+        <v>3060</v>
       </c>
       <c r="J2" s="3">
-        <v>3372.0</v>
+        <v>3372</v>
       </c>
       <c r="K2" s="3">
-        <v>2936.0</v>
+        <v>2936</v>
       </c>
       <c r="L2" s="3">
-        <v>3116.0</v>
+        <v>3116</v>
       </c>
       <c r="M2" s="3">
-        <v>2991.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B3" s="3">
-        <v>5540268.0</v>
+        <v>5540268</v>
       </c>
       <c r="C3" s="3">
-        <v>5773652.0</v>
+        <v>5773652</v>
       </c>
       <c r="D3" s="3">
-        <v>4352554.0</v>
+        <v>4352554</v>
       </c>
       <c r="E3" s="3">
-        <v>4178918.0</v>
+        <v>4178918</v>
       </c>
       <c r="F3" s="3">
-        <v>4301892.0</v>
+        <v>4301892</v>
       </c>
       <c r="G3" s="3">
-        <v>3007.0</v>
+        <v>3007</v>
       </c>
       <c r="H3" s="3">
-        <v>3122.0</v>
+        <v>3122</v>
       </c>
       <c r="I3" s="3">
-        <v>2891.0</v>
+        <v>2891</v>
       </c>
       <c r="J3" s="3">
-        <v>3267.0</v>
+        <v>3267</v>
       </c>
       <c r="K3" s="3">
-        <v>3044.0</v>
+        <v>3044</v>
       </c>
       <c r="L3" s="3">
-        <v>3247.0</v>
+        <v>3247</v>
       </c>
       <c r="M3" s="3">
-        <v>3418.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="3">
-        <v>3677115.0</v>
+        <v>3677115</v>
       </c>
       <c r="C4" s="3">
-        <v>3643783.0</v>
+        <v>3643783</v>
       </c>
       <c r="D4" s="3">
-        <v>311334.0</v>
+        <v>311334</v>
       </c>
       <c r="E4" s="3">
-        <v>398350.0</v>
+        <v>398350</v>
       </c>
       <c r="F4" s="3">
-        <v>333065.0</v>
+        <v>333065</v>
       </c>
       <c r="G4" s="3">
-        <v>3052.0</v>
+        <v>3052</v>
       </c>
       <c r="H4" s="3">
-        <v>3057.0</v>
+        <v>3057</v>
       </c>
       <c r="I4" s="3">
-        <v>3188.0</v>
+        <v>3188</v>
       </c>
       <c r="J4" s="3">
-        <v>2943.0</v>
+        <v>2943</v>
       </c>
       <c r="K4" s="3">
-        <v>3147.0</v>
+        <v>3147</v>
       </c>
       <c r="L4" s="3">
-        <v>3607.0</v>
+        <v>3607</v>
       </c>
       <c r="M4" s="3">
-        <v>4039.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4039</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="3">
-        <v>3132476.0</v>
+        <v>3132476</v>
       </c>
       <c r="C5" s="3">
-        <v>2986983.0</v>
+        <v>2986983</v>
       </c>
       <c r="D5" s="3">
-        <v>1596425.0</v>
+        <v>1596425</v>
       </c>
       <c r="E5" s="3">
-        <v>1621894.0</v>
+        <v>1621894</v>
       </c>
       <c r="F5" s="3">
-        <v>1637300.0</v>
+        <v>1637300</v>
       </c>
       <c r="G5" s="3">
-        <v>3266.0</v>
+        <v>3266</v>
       </c>
       <c r="H5" s="3">
-        <v>3341.0</v>
+        <v>3341</v>
       </c>
       <c r="I5" s="3">
-        <v>3236.0</v>
+        <v>3236</v>
       </c>
       <c r="J5" s="3">
-        <v>2929.0</v>
+        <v>2929</v>
       </c>
       <c r="K5" s="3">
-        <v>3646.0</v>
+        <v>3646</v>
       </c>
       <c r="L5" s="3">
-        <v>3499.0</v>
+        <v>3499</v>
       </c>
       <c r="M5" s="3">
-        <v>2712.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="3">
-        <v>2409478.0</v>
+        <v>2409478</v>
       </c>
       <c r="C6" s="3">
-        <v>2266942.0</v>
+        <v>2266942</v>
       </c>
       <c r="D6" s="3">
-        <v>3198.0</v>
+        <v>3198</v>
       </c>
       <c r="E6" s="3">
-        <v>2949.0</v>
+        <v>2949</v>
       </c>
       <c r="F6" s="3">
-        <v>2799.0</v>
+        <v>2799</v>
       </c>
       <c r="G6" s="3">
-        <v>2898.0</v>
+        <v>2898</v>
       </c>
       <c r="H6" s="3">
-        <v>3392.0</v>
+        <v>3392</v>
       </c>
       <c r="I6" s="3">
-        <v>3172.0</v>
+        <v>3172</v>
       </c>
       <c r="J6" s="3">
-        <v>3061.0</v>
+        <v>3061</v>
       </c>
       <c r="K6" s="3">
-        <v>2891.0</v>
+        <v>2891</v>
       </c>
       <c r="L6" s="3">
-        <v>3018.0</v>
+        <v>3018</v>
       </c>
       <c r="M6" s="3">
-        <v>2763.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B7" s="3">
-        <v>1570284.0</v>
+        <v>1570284</v>
       </c>
       <c r="C7" s="3">
-        <v>1607156.0</v>
+        <v>1607156</v>
       </c>
       <c r="D7" s="3">
-        <v>3270.0</v>
+        <v>3270</v>
       </c>
       <c r="E7" s="3">
-        <v>2736.0</v>
+        <v>2736</v>
       </c>
       <c r="F7" s="3">
-        <v>2610.0</v>
+        <v>2610</v>
       </c>
       <c r="G7" s="3">
-        <v>2891.0</v>
+        <v>2891</v>
       </c>
       <c r="H7" s="3">
-        <v>3207.0</v>
+        <v>3207</v>
       </c>
       <c r="I7" s="3">
-        <v>2944.0</v>
+        <v>2944</v>
       </c>
       <c r="J7" s="3">
-        <v>3183.0</v>
+        <v>3183</v>
       </c>
       <c r="K7" s="3">
-        <v>2777.0</v>
+        <v>2777</v>
       </c>
       <c r="L7" s="3">
-        <v>2877.0</v>
+        <v>2877</v>
       </c>
       <c r="M7" s="3">
-        <v>3093.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="3">
-        <v>866225.0</v>
+        <v>866225</v>
       </c>
       <c r="C8" s="3">
-        <v>828070.0</v>
+        <v>828070</v>
       </c>
       <c r="D8" s="3">
-        <v>3654.0</v>
+        <v>3654</v>
       </c>
       <c r="E8" s="3">
-        <v>3375.0</v>
+        <v>3375</v>
       </c>
       <c r="F8" s="3">
-        <v>2978.0</v>
+        <v>2978</v>
       </c>
       <c r="G8" s="3">
-        <v>3078.0</v>
+        <v>3078</v>
       </c>
       <c r="H8" s="3">
-        <v>3140.0</v>
+        <v>3140</v>
       </c>
       <c r="I8" s="3">
-        <v>3185.0</v>
+        <v>3185</v>
       </c>
       <c r="J8" s="3">
-        <v>3348.0</v>
+        <v>3348</v>
       </c>
       <c r="K8" s="3">
-        <v>2996.0</v>
+        <v>2996</v>
       </c>
       <c r="L8" s="3">
-        <v>3405.0</v>
+        <v>3405</v>
       </c>
       <c r="M8" s="3">
-        <v>3129.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="3">
-        <v>41111.0</v>
+        <v>41111</v>
       </c>
       <c r="C9" s="3">
-        <v>40222.0</v>
+        <v>40222</v>
       </c>
       <c r="D9" s="3">
-        <v>2894.0</v>
+        <v>2894</v>
       </c>
       <c r="E9" s="3">
-        <v>3181.0</v>
+        <v>3181</v>
       </c>
       <c r="F9" s="3">
-        <v>3350.0</v>
+        <v>3350</v>
       </c>
       <c r="G9" s="3">
-        <v>3011.0</v>
+        <v>3011</v>
       </c>
       <c r="H9" s="3">
-        <v>3302.0</v>
+        <v>3302</v>
       </c>
       <c r="I9" s="3">
-        <v>3368.0</v>
+        <v>3368</v>
       </c>
       <c r="J9" s="3">
-        <v>3530.0</v>
+        <v>3530</v>
       </c>
       <c r="K9" s="3">
-        <v>3071.0</v>
+        <v>3071</v>
       </c>
       <c r="L9" s="3">
-        <v>3043.0</v>
+        <v>3043</v>
       </c>
       <c r="M9" s="3">
-        <v>3508.0</v>
+        <v>3508</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="39.6">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="3">
+        <v>7983909</v>
+      </c>
+      <c r="C2" s="3">
+        <v>7564875</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4650965</v>
+      </c>
+      <c r="E2" s="3">
+        <v>4291172</v>
+      </c>
+      <c r="F2" s="3">
+        <v>4430788</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3019</v>
+      </c>
+      <c r="H2" s="3">
+        <v>3710</v>
+      </c>
+      <c r="I2" s="3">
+        <v>3060</v>
+      </c>
+      <c r="J2" s="3">
+        <v>3372</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2936</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3116</v>
+      </c>
+      <c r="M2" s="3">
+        <v>2991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5540268</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5773652</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4352554</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4178918</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4301892</v>
+      </c>
+      <c r="G3" s="3">
+        <v>3007</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3122</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2891</v>
+      </c>
+      <c r="J3" s="3">
+        <v>3267</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3044</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3247</v>
+      </c>
+      <c r="M3" s="3">
+        <v>3418</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3677115</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3643783</v>
+      </c>
+      <c r="D4" s="3">
+        <v>311334</v>
+      </c>
+      <c r="E4" s="3">
+        <v>398350</v>
+      </c>
+      <c r="F4" s="3">
+        <v>333065</v>
+      </c>
+      <c r="G4" s="3">
+        <v>3052</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3057</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3188</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2943</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3147</v>
+      </c>
+      <c r="L4" s="3">
+        <v>3607</v>
+      </c>
+      <c r="M4" s="3">
+        <v>4039</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3132476</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2986983</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1596425</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1621894</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1637300</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3266</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3341</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3236</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2929</v>
+      </c>
+      <c r="K5" s="3">
+        <v>3646</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3499</v>
+      </c>
+      <c r="M5" s="3">
+        <v>2712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2409478</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2266942</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3198</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2949</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2799</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2898</v>
+      </c>
+      <c r="H6" s="3">
+        <v>3392</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3172</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3061</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2891</v>
+      </c>
+      <c r="L6" s="3">
+        <v>3018</v>
+      </c>
+      <c r="M6" s="3">
+        <v>2763</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1570284</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1607156</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3270</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2736</v>
+      </c>
+      <c r="F7" s="3">
+        <v>2610</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2891</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3207</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2944</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3183</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2777</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2877</v>
+      </c>
+      <c r="M7" s="3">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="3">
+        <v>866225</v>
+      </c>
+      <c r="C8" s="3">
+        <v>828070</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3654</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3375</v>
+      </c>
+      <c r="F8" s="3">
+        <v>2978</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3078</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3140</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3185</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3348</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2996</v>
+      </c>
+      <c r="L8" s="3">
+        <v>3405</v>
+      </c>
+      <c r="M8" s="3">
+        <v>3129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="3">
+        <v>41111</v>
+      </c>
+      <c r="C9" s="3">
+        <v>40222</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2894</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3181</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3350</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3011</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3302</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3368</v>
+      </c>
+      <c r="J9" s="3">
+        <v>3530</v>
+      </c>
+      <c r="K9" s="3">
+        <v>3071</v>
+      </c>
+      <c r="L9" s="3">
+        <v>3043</v>
+      </c>
+      <c r="M9" s="3">
+        <v>3508</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>